<commit_message>
chnges before moving to dropwizard
</commit_message>
<xml_diff>
--- a/AccountsModule/Tasks.xlsx
+++ b/AccountsModule/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\Java\Tweeter\AccountsModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30AA4A4-90B0-4D4B-A4B3-3F8D2A955712}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D000C966-89A8-4109-96FF-BE4BAA66CB3C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="23686" windowHeight="14586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Status</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>DB Integration</t>
+  </si>
+  <si>
+    <t>Integrate Dropwizard</t>
   </si>
 </sst>
 </file>
@@ -450,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H12"/>
+  <dimension ref="A2:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -548,6 +551,11 @@
       </c>
       <c r="B12" s="5"/>
     </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>